<commit_message>
Filtered results by BOEM WEAs and integrated two different species sets
</commit_message>
<xml_diff>
--- a/OSW_spp_set.xlsx
+++ b/OSW_spp_set.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/curt.whitmire/Documents/GitHub/SurveyCoverage/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD3CE960-E5B6-F847-923F-7DA5145AB7DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CC5C821-17BD-8B41-BA78-60CDF5B6CD48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6280" yWindow="460" windowWidth="34600" windowHeight="25940" xr2:uid="{55A5CB8E-7C98-EB4B-917D-42EEC5CD5314}"/>
+    <workbookView xWindow="1660" yWindow="460" windowWidth="47720" windowHeight="25940" activeTab="1" xr2:uid="{55A5CB8E-7C98-EB4B-917D-42EEC5CD5314}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="spp_of_interest" sheetId="1" r:id="rId1"/>
+    <sheet name="FMP" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="291">
   <si>
     <t>sablefish</t>
   </si>
@@ -318,13 +319,601 @@
   </si>
   <si>
     <t>Pacific spiny dogfish</t>
+  </si>
+  <si>
+    <t>lat_max</t>
+  </si>
+  <si>
+    <t>lat_min</t>
+  </si>
+  <si>
+    <t>dep_min</t>
+  </si>
+  <si>
+    <t>dep_max</t>
+  </si>
+  <si>
+    <t>Arrowtooth Flounder</t>
+  </si>
+  <si>
+    <t>Atheresthes stomias</t>
+  </si>
+  <si>
+    <t>Butter Sole</t>
+  </si>
+  <si>
+    <t>Isopsetta isolepis</t>
+  </si>
+  <si>
+    <t>Curlfin Sole</t>
+  </si>
+  <si>
+    <t>Pleuronichthys decurrens</t>
+  </si>
+  <si>
+    <t>Dover Sole</t>
+  </si>
+  <si>
+    <t>Microstomus pacificus</t>
+  </si>
+  <si>
+    <t>English Sole</t>
+  </si>
+  <si>
+    <t>Parophrys vetulus</t>
+  </si>
+  <si>
+    <t>Flathead Sole</t>
+  </si>
+  <si>
+    <t>Hippoglossoides elassodon</t>
+  </si>
+  <si>
+    <t>Pacific Sanddab</t>
+  </si>
+  <si>
+    <t>Citharichthys sordidus</t>
+  </si>
+  <si>
+    <t>Petrale Sole</t>
+  </si>
+  <si>
+    <t>Eopsetta jordani</t>
+  </si>
+  <si>
+    <t>Rex Sole</t>
+  </si>
+  <si>
+    <t>Glyptocephalus zachirus</t>
+  </si>
+  <si>
+    <t>Sand Sole</t>
+  </si>
+  <si>
+    <t>Psettichthys melanostictus</t>
+  </si>
+  <si>
+    <t>Rock Sole</t>
+  </si>
+  <si>
+    <t>Lepidopsetta bilineata</t>
+  </si>
+  <si>
+    <t>Starry Flounder</t>
+  </si>
+  <si>
+    <t>Platichthys stellatus</t>
+  </si>
+  <si>
+    <t>Aurora Rockfish</t>
+  </si>
+  <si>
+    <t>Sebastes aurora</t>
+  </si>
+  <si>
+    <t>Bank Rockfish</t>
+  </si>
+  <si>
+    <t>Black Rockfish</t>
+  </si>
+  <si>
+    <t>Black-And-Yellow Rockfish</t>
+  </si>
+  <si>
+    <t>Blackgill Rockfish</t>
+  </si>
+  <si>
+    <t>Blue Rockfish</t>
+  </si>
+  <si>
+    <t>Bocaccio</t>
+  </si>
+  <si>
+    <t>Bronzespotted Rockfish</t>
+  </si>
+  <si>
+    <t>Brown Rockfish</t>
+  </si>
+  <si>
+    <t>Calico Rockfish</t>
+  </si>
+  <si>
+    <t>California scorpionfish</t>
+  </si>
+  <si>
+    <t>Scorpaena guttata</t>
+  </si>
+  <si>
+    <t>Canary Rockfish</t>
+  </si>
+  <si>
+    <t>Chameleon Rockfish</t>
+  </si>
+  <si>
+    <t>Chilipepper</t>
+  </si>
+  <si>
+    <t>China Rockfish</t>
+  </si>
+  <si>
+    <t>Copper Rockfish</t>
+  </si>
+  <si>
+    <t>Cowcod</t>
+  </si>
+  <si>
+    <t>Darkblotched Rockfish</t>
+  </si>
+  <si>
+    <t>Dusky Rockfish</t>
+  </si>
+  <si>
+    <t>Flag Rockfish</t>
+  </si>
+  <si>
+    <t>Gopher Rockfish</t>
+  </si>
+  <si>
+    <t>Grass Rockfish</t>
+  </si>
+  <si>
+    <t>Greenblotched Rockfish</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>flatfish</t>
+  </si>
+  <si>
+    <t>Greenspotted Rockfish</t>
+  </si>
+  <si>
+    <t>Greenstriped Rockfish</t>
+  </si>
+  <si>
+    <t>Harlequin Rockfish</t>
+  </si>
+  <si>
+    <t>Honeycomb Rockfish</t>
+  </si>
+  <si>
+    <t>Kelp Rockfish</t>
+  </si>
+  <si>
+    <t>Longspine Thornyhead</t>
+  </si>
+  <si>
+    <t>Sebastolobus altivelis</t>
+  </si>
+  <si>
+    <t>Mexican Rockfish</t>
+  </si>
+  <si>
+    <t>Olive Rockfish</t>
+  </si>
+  <si>
+    <t>Pacific Ocean Perch</t>
+  </si>
+  <si>
+    <t>Pink Rockfish</t>
+  </si>
+  <si>
+    <t>Puget Sound Rockfish</t>
+  </si>
+  <si>
+    <t>Pygmy Rockfish</t>
+  </si>
+  <si>
+    <t>Quillback Rockfish</t>
+  </si>
+  <si>
+    <t>Scorpaenodes xyris</t>
+  </si>
+  <si>
+    <t>Redbanded Rockfish</t>
+  </si>
+  <si>
+    <t>Redstripe Rockfish</t>
+  </si>
+  <si>
+    <t>Rosethorn Rockfish</t>
+  </si>
+  <si>
+    <t>Rosy Rockfish</t>
+  </si>
+  <si>
+    <t>Rougheye Rockfish</t>
+  </si>
+  <si>
+    <t>Sharpchin Rockfish</t>
+  </si>
+  <si>
+    <t>Shortbelly Rockfish</t>
+  </si>
+  <si>
+    <t>Shortraker Rockfish</t>
+  </si>
+  <si>
+    <t>Shortspine Thornyhead</t>
+  </si>
+  <si>
+    <t>Sebastolobus alascanus</t>
+  </si>
+  <si>
+    <t>Silvergray Rockfish</t>
+  </si>
+  <si>
+    <t>Speckled Rockfish</t>
+  </si>
+  <si>
+    <t>Splitnose Rockfish</t>
+  </si>
+  <si>
+    <t>Squarespot Rockfish</t>
+  </si>
+  <si>
+    <t>Starry Rockfish</t>
+  </si>
+  <si>
+    <t>Scorpaena mystes</t>
+  </si>
+  <si>
+    <t>Stripetail Rockfish</t>
+  </si>
+  <si>
+    <t>Tiger Rockfish</t>
+  </si>
+  <si>
+    <t>Treefish</t>
+  </si>
+  <si>
+    <t>Vermilion Rockfish</t>
+  </si>
+  <si>
+    <t>Widow Rockfish</t>
+  </si>
+  <si>
+    <t>Yelloweye Rockfish</t>
+  </si>
+  <si>
+    <t>Yellowmouth Rockfish</t>
+  </si>
+  <si>
+    <t>Yellowtail Rockfish</t>
+  </si>
+  <si>
+    <t>Cabezon</t>
+  </si>
+  <si>
+    <t>Scorpaenichthys marmoratus</t>
+  </si>
+  <si>
+    <t>roundfish</t>
+  </si>
+  <si>
+    <t>Kelp Greenling</t>
+  </si>
+  <si>
+    <t>Hexagrammos decagrammus</t>
+  </si>
+  <si>
+    <t>Lingcod</t>
+  </si>
+  <si>
+    <t>Ophiodon elongatus</t>
+  </si>
+  <si>
+    <t>Pacific Cod</t>
+  </si>
+  <si>
+    <t>Gadus macrocephalus</t>
+  </si>
+  <si>
+    <t>Merluccius productus</t>
+  </si>
+  <si>
+    <t>Sablefish</t>
+  </si>
+  <si>
+    <t>Anoplopoma fimbria</t>
+  </si>
+  <si>
+    <t>Big Skate</t>
+  </si>
+  <si>
+    <t>Leopard Shark</t>
+  </si>
+  <si>
+    <t>Triakis semifasciata</t>
+  </si>
+  <si>
+    <t>Longnose Skate</t>
+  </si>
+  <si>
+    <t>Raja rhina</t>
+  </si>
+  <si>
+    <t>Pacific Spiny Dogfish</t>
+  </si>
+  <si>
+    <t>Squalus suckleyi</t>
+  </si>
+  <si>
+    <t>elasmobranch</t>
+  </si>
+  <si>
+    <t>Blackspotted Rockfish</t>
+  </si>
+  <si>
+    <t>Deacon Rockfish</t>
+  </si>
+  <si>
+    <t>Dwarf-Red Rockfish</t>
+  </si>
+  <si>
+    <t>Freckled Rockfish</t>
+  </si>
+  <si>
+    <t>Halfbanded Rockfish</t>
+  </si>
+  <si>
+    <t>Rainbow scorpionfish</t>
+  </si>
+  <si>
+    <t>Semaphore Rockfish</t>
+  </si>
+  <si>
+    <t>Pinkrose Rockfish</t>
+  </si>
+  <si>
+    <t>Stone Scorpionfish</t>
+  </si>
+  <si>
+    <t>Sunset Rockfish</t>
+  </si>
+  <si>
+    <t>Swordspine Rockfish</t>
+  </si>
+  <si>
+    <t>Whitespotted Rockfish</t>
+  </si>
+  <si>
+    <t>Pacific hake</t>
+  </si>
+  <si>
+    <t>Sebastes rufus</t>
+  </si>
+  <si>
+    <t>Sebastes melanops</t>
+  </si>
+  <si>
+    <t>Sebastes chrysomelas</t>
+  </si>
+  <si>
+    <t>Sebastes melanostomus</t>
+  </si>
+  <si>
+    <t>Sebastes melanostictus</t>
+  </si>
+  <si>
+    <t>Sebastes mystinus</t>
+  </si>
+  <si>
+    <t>Sebastes paucispinis</t>
+  </si>
+  <si>
+    <t>Sebastes gilli</t>
+  </si>
+  <si>
+    <t>Sebastes auriculatus</t>
+  </si>
+  <si>
+    <t>Sebastes dallii</t>
+  </si>
+  <si>
+    <t>Sebastes pinniger</t>
+  </si>
+  <si>
+    <t>Sebastes phillipsi</t>
+  </si>
+  <si>
+    <t>Sebastes goodei</t>
+  </si>
+  <si>
+    <t>Sebastes nebulosus</t>
+  </si>
+  <si>
+    <t>Sebastes caurinus</t>
+  </si>
+  <si>
+    <t>Sebastes levis</t>
+  </si>
+  <si>
+    <t>Sebastes crameri</t>
+  </si>
+  <si>
+    <t>Sebastes diaconus</t>
+  </si>
+  <si>
+    <t>Sebastes variabilis</t>
+  </si>
+  <si>
+    <t>Sebastes rufinanus</t>
+  </si>
+  <si>
+    <t>Sebastes rubrivinctus</t>
+  </si>
+  <si>
+    <t>Sebastes lentiginosus</t>
+  </si>
+  <si>
+    <t>Sebastes carnatus</t>
+  </si>
+  <si>
+    <t>Sebastes rastrelliger</t>
+  </si>
+  <si>
+    <t>Sebastes rosenblatti</t>
+  </si>
+  <si>
+    <t>Sebastes chlorostictus</t>
+  </si>
+  <si>
+    <t>Sebastes elongatus</t>
+  </si>
+  <si>
+    <t>Sebastes semicinctus</t>
+  </si>
+  <si>
+    <t>Sebastes variegatus</t>
+  </si>
+  <si>
+    <t>Sebastes umbrosus</t>
+  </si>
+  <si>
+    <t>Sebastes atrovirens</t>
+  </si>
+  <si>
+    <t>Sebastes macdonaldi</t>
+  </si>
+  <si>
+    <t>Sebastes serranoides</t>
+  </si>
+  <si>
+    <t>Sebastes alutus</t>
+  </si>
+  <si>
+    <t>Sebastes eos</t>
+  </si>
+  <si>
+    <t>Sebastes simulator</t>
+  </si>
+  <si>
+    <t>Sebastes emphaeus</t>
+  </si>
+  <si>
+    <t>Sebastes wilsoni</t>
+  </si>
+  <si>
+    <t>Sebastes maliger</t>
+  </si>
+  <si>
+    <t>Sebastes babcocki</t>
+  </si>
+  <si>
+    <t>Sebastes proriger</t>
+  </si>
+  <si>
+    <t>Sebastes helvomaculatus</t>
+  </si>
+  <si>
+    <t>Sebastes rosaceus</t>
+  </si>
+  <si>
+    <t>Sebastes aleutianus</t>
+  </si>
+  <si>
+    <t>Sebastes melanosema</t>
+  </si>
+  <si>
+    <t>Sebastes zacentrus</t>
+  </si>
+  <si>
+    <t>Sebastes jordani</t>
+  </si>
+  <si>
+    <t>Sebastes borealis</t>
+  </si>
+  <si>
+    <t>Sebastes brevispinis</t>
+  </si>
+  <si>
+    <t>Sebastes ovalis</t>
+  </si>
+  <si>
+    <t>Sebastes diploproa</t>
+  </si>
+  <si>
+    <t>Sebastes hopkinsi</t>
+  </si>
+  <si>
+    <t>Sebastes constellatus</t>
+  </si>
+  <si>
+    <t>Sebastes saxicola</t>
+  </si>
+  <si>
+    <t>Sebastes crocotulus</t>
+  </si>
+  <si>
+    <t>Sebastes ensifer</t>
+  </si>
+  <si>
+    <t>Sebastes nigrocinctus</t>
+  </si>
+  <si>
+    <t>Sebastes serriceps</t>
+  </si>
+  <si>
+    <t>Sebastes miniatus</t>
+  </si>
+  <si>
+    <t>Sebastes moseri</t>
+  </si>
+  <si>
+    <t>Sebastes entomelas</t>
+  </si>
+  <si>
+    <t>Sebastes ruberrimus</t>
+  </si>
+  <si>
+    <t>Sebastes reedi</t>
+  </si>
+  <si>
+    <t>Sebastes flavidus</t>
+  </si>
+  <si>
+    <t>FMP</t>
+  </si>
+  <si>
+    <t>groundfish</t>
+  </si>
+  <si>
+    <t>Common_Name</t>
+  </si>
+  <si>
+    <t>Scientific_Name</t>
+  </si>
+  <si>
+    <t>Raja binoculata</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -347,8 +936,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -371,6 +973,12 @@
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -399,12 +1007,26 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="20% - Accent2" xfId="2" builtinId="34"/>
@@ -723,10 +1345,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D89D029-2C34-B349-87A1-97E86D5B773E}">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView zoomScale="200" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -740,7 +1362,7 @@
     <col min="7" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>43</v>
       </c>
@@ -765,8 +1387,20 @@
       <c r="H1" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="I1" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -786,8 +1420,20 @@
       <c r="F2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I2">
+        <v>23</v>
+      </c>
+      <c r="J2">
+        <v>64</v>
+      </c>
+      <c r="K2">
+        <v>175</v>
+      </c>
+      <c r="L2">
+        <v>2740</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -811,7 +1457,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -835,7 +1481,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -859,7 +1505,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -883,7 +1529,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -907,7 +1553,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -931,7 +1577,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -952,7 +1598,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -976,7 +1622,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1000,7 +1646,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1027,7 +1673,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1051,7 +1697,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1075,7 +1721,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1098,8 +1744,20 @@
       <c r="G15" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I15">
+        <v>32</v>
+      </c>
+      <c r="J15">
+        <v>70</v>
+      </c>
+      <c r="K15">
+        <v>25</v>
+      </c>
+      <c r="L15">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1345,4 +2003,1329 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6799F3A-AC7C-904A-9585-9105FC4F3813}">
+  <dimension ref="A1:D94"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.83203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" style="6" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>289</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="D2" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="D3" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="D4" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="D5" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="D6" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="D7" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="D8" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="D9" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="D10" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="D11" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="D12" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="D13" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>238</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D39" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D40" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D41" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D43" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D44" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D45" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="C46" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D46" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="C47" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D47" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="C48" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D48" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="C49" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D49" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="C50" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D50" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="C51" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D51" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="C52" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D52" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="C53" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D53" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="C54" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D54" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="C55" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D55" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="C56" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D56" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="C57" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D57" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="B58" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="C58" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D58" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="C59" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D59" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="B60" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="C60" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D60" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B61" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="C61" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D61" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="B62" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="C62" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D62" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="B63" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="C63" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D63" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="B64" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="C64" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D64" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="B65" s="9" t="s">
+        <v>269</v>
+      </c>
+      <c r="C65" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D65" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="B66" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="C66" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D66" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="B67" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="C67" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D67" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="B68" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="C68" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D68" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="B69" s="9" t="s">
+        <v>272</v>
+      </c>
+      <c r="C69" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D69" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="B70" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="C70" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D70" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="B71" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="C71" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D71" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="B72" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="C72" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D72" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="B73" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="C73" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D73" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="B74" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="C74" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D74" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="B75" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="C75" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D75" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="B76" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="C76" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D76" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B77" s="9" t="s">
+        <v>279</v>
+      </c>
+      <c r="C77" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D77" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="B78" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="C78" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D78" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="B79" s="9" t="s">
+        <v>281</v>
+      </c>
+      <c r="C79" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D79" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="B80" s="9" t="s">
+        <v>282</v>
+      </c>
+      <c r="C80" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D80" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="B81" s="9" t="s">
+        <v>283</v>
+      </c>
+      <c r="C81" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D81" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="B82" s="9" t="s">
+        <v>284</v>
+      </c>
+      <c r="C82" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D82" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="B83" s="9" t="s">
+        <v>285</v>
+      </c>
+      <c r="C83" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D83" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="B84" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="C84" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="D84" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="B85" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="C85" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="D85" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="B86" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="C86" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="D86" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="B87" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="C87" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="D87" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="B88" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="C88" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="D88" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="B89" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="C89" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="D89" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="B90" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="C90" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="D90" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="B91" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="C91" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="D91" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="B92" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="C92" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="D92" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="B93" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="C93" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="D93" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A94" s="10"/>
+      <c r="B94" s="10"/>
+      <c r="C94" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>